<commit_message>
Added tests for IT6
</commit_message>
<xml_diff>
--- a/Integrationsplan_Updated.xlsx
+++ b/Integrationsplan_Updated.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\4semester\SWT25_Assignment3_Microwave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trill\OneDrive\Skrivebord\SWT SOURCE\Microwave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41A7BB1-F50E-44FD-A0A6-6EEA28E9B0D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA70961-B420-4689-AB10-F58CB5BF2EEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="10140" xr2:uid="{A94110E4-C87A-4C65-9E94-07A2885B6C0F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="24">
   <si>
     <t>Step #</t>
   </si>
@@ -568,12 +568,15 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="63.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +615,7 @@
       </c>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -647,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -682,7 +685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -717,7 +720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -752,7 +755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>2</v>
       </c>
@@ -791,7 +794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -830,7 +833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -864,7 +867,9 @@
       <c r="K8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="M8" s="9" t="s">
         <v>19</v>
       </c>
@@ -872,7 +877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -906,7 +911,9 @@
       <c r="K9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="M9" s="4" t="s">
         <v>20</v>
       </c>
@@ -914,9 +921,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>12</v>
@@ -955,9 +962,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>12</v>
@@ -996,9 +1003,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -1037,7 +1044,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1052,7 +1059,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1067,7 +1074,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1082,7 +1089,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1097,7 +1104,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1112,7 +1119,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="14"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E21" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some tests for Door_Button_Display and updated integrationplan
</commit_message>
<xml_diff>
--- a/Integrationsplan_Updated.xlsx
+++ b/Integrationsplan_Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trill\OneDrive\Skrivebord\SWT SOURCE\Microwave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA70961-B420-4689-AB10-F58CB5BF2EEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF2E50D-3F53-4347-B31F-D2FDA6C4201B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="10140" xr2:uid="{A94110E4-C87A-4C65-9E94-07A2885B6C0F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="25">
   <si>
     <t>Step #</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mellem step 5 og step 6 ved jeg ikke hvordan vi beskriver, da det er de samme klasser der er stubs og drivere, der gås bare tilbage i hierarket(andre functioner bliver kaldt). </t>
+  </si>
+  <si>
+    <t>I gang med dette (TM)</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,6 +963,9 @@
       </c>
       <c r="M10" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>